<commit_message>
add definition of paper and honor.
</commit_message>
<xml_diff>
--- a/附件4 竞聘人选情况表-计算机.xlsx
+++ b/附件4 竞聘人选情况表-计算机.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\stidb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66060E18-6EE9-46B6-B3C7-48F353F2DC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88D693F-AC44-451E-8C87-3A4CEC78BCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,13 +190,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">标准：无
-专利：
-软件著作权（技术秘密）：
-</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>{{data.sap}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -212,6 +205,22 @@
       获奖时间：{{pr.year}}年
 {% endfor %}</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">标准：无
+专利：
+{% for pa in data.patents -%}   
+{{ loop.index }}.{{ pa.patent_name }}，{{pa.status}}，
+{%- if pa.status == '授权有效' -%}
+授权日：{{pa.grant_date}}，专利号：{{pa.patent_code}} ,
+{%- else -%}
+申请日：{{pa.apply_date}}，申请号：{{pa.apply_code}} ,
+{%- endif -%}
+排名：第{{pa.person_rank}}
+{% endfor %}
+软件著作权（技术秘密）：
+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -574,36 +583,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -613,6 +592,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -666,6 +648,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -678,12 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -708,6 +687,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1015,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:L17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7:W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.15"/>
@@ -1052,62 +1061,62 @@
       <c r="A1" s="2"/>
     </row>
     <row r="2" spans="1:25" s="5" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
     </row>
     <row r="3" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="57"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
     </row>
     <row r="4" spans="1:25" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
@@ -1119,45 +1128,45 @@
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="51"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="51"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="28" t="s">
+      <c r="L4" s="43"/>
+      <c r="M4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="58"/>
+      <c r="N4" s="48"/>
       <c r="O4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="51"/>
-      <c r="S4" s="28" t="s">
+      <c r="R4" s="43"/>
+      <c r="S4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="58"/>
+      <c r="T4" s="48"/>
       <c r="U4" s="6" t="s">
         <v>13</v>
       </c>
@@ -1176,10 +1185,10 @@
     </row>
     <row r="5" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>38</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -1191,14 +1200,14 @@
       <c r="J5" s="11"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="60"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="50"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="60"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="50"/>
       <c r="U5" s="11"/>
       <c r="V5" s="13"/>
       <c r="W5" s="14"/>
@@ -1206,533 +1215,533 @@
       <c r="Y5" s="11"/>
     </row>
     <row r="6" spans="1:25" s="4" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="28" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="51" t="s">
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="51"/>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="51"/>
-      <c r="X6" s="26" t="s">
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="43"/>
+      <c r="X6" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="Y6" s="26"/>
+      <c r="Y6" s="39"/>
     </row>
     <row r="7" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="53"/>
-      <c r="Y7" s="47"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="36"/>
+      <c r="X7" s="52"/>
+      <c r="Y7" s="38"/>
     </row>
     <row r="8" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="47"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="38"/>
     </row>
     <row r="9" spans="1:25" ht="40.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="45"/>
-      <c r="W9" s="45"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="47"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="36"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
     </row>
     <row r="10" spans="1:25" ht="47.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="45"/>
-      <c r="W10" s="45"/>
-      <c r="X10" s="47"/>
-      <c r="Y10" s="47"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
     </row>
     <row r="11" spans="1:25" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="45"/>
-      <c r="V11" s="45"/>
-      <c r="W11" s="45"/>
-      <c r="X11" s="47"/>
-      <c r="Y11" s="47"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
     </row>
     <row r="12" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="38" t="s">
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="45"/>
-      <c r="V12" s="45"/>
-      <c r="W12" s="45"/>
-      <c r="X12" s="47"/>
-      <c r="Y12" s="47"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
     </row>
     <row r="13" spans="1:25" ht="161.44999999999999" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="45"/>
-      <c r="W13" s="45"/>
-      <c r="X13" s="47"/>
-      <c r="Y13" s="47"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
     </row>
     <row r="14" spans="1:25" s="4" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26" t="s">
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26" t="s">
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="Y14" s="26"/>
+      <c r="Y14" s="39"/>
     </row>
     <row r="15" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="45" t="s">
+      <c r="A15" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="46" t="s">
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="T15" s="47"/>
-      <c r="U15" s="47"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="47"/>
-      <c r="X15" s="44" t="s">
+      <c r="T15" s="38"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="38"/>
+      <c r="X15" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="Y15" s="45"/>
+      <c r="Y15" s="36"/>
     </row>
     <row r="16" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="47"/>
-      <c r="T16" s="47"/>
-      <c r="U16" s="47"/>
-      <c r="V16" s="47"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="45"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="38"/>
+      <c r="U16" s="38"/>
+      <c r="V16" s="38"/>
+      <c r="W16" s="38"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="36"/>
     </row>
     <row r="17" spans="1:25" ht="363.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="47"/>
-      <c r="T17" s="47"/>
-      <c r="U17" s="47"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="47"/>
-      <c r="T18" s="47"/>
-      <c r="U18" s="47"/>
-      <c r="V18" s="47"/>
-      <c r="W18" s="47"/>
-      <c r="X18" s="45"/>
-      <c r="Y18" s="45"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
     </row>
     <row r="19" spans="1:25" ht="40.9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="47"/>
-      <c r="T19" s="47"/>
-      <c r="U19" s="47"/>
-      <c r="V19" s="47"/>
-      <c r="W19" s="47"/>
-      <c r="X19" s="45"/>
-      <c r="Y19" s="45"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
     </row>
     <row r="20" spans="1:25" ht="40.9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="47"/>
-      <c r="T20" s="47"/>
-      <c r="U20" s="47"/>
-      <c r="V20" s="47"/>
-      <c r="W20" s="47"/>
-      <c r="X20" s="45"/>
-      <c r="Y20" s="45"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="36"/>
     </row>
     <row r="21" spans="1:25" ht="44.65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="47"/>
-      <c r="V21" s="47"/>
-      <c r="W21" s="47"/>
-      <c r="X21" s="45"/>
-      <c r="Y21" s="45"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="36"/>
     </row>
     <row r="22" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="47"/>
-      <c r="T22" s="47"/>
-      <c r="U22" s="47"/>
-      <c r="V22" s="47"/>
-      <c r="W22" s="47"/>
-      <c r="X22" s="45"/>
-      <c r="Y22" s="45"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="38"/>
+      <c r="T22" s="38"/>
+      <c r="U22" s="38"/>
+      <c r="V22" s="38"/>
+      <c r="W22" s="38"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36"/>
     </row>
     <row r="23" spans="1:25" ht="175.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="S23" s="47"/>
-      <c r="T23" s="47"/>
-      <c r="U23" s="47"/>
-      <c r="V23" s="47"/>
-      <c r="W23" s="47"/>
-      <c r="X23" s="45"/>
-      <c r="Y23" s="45"/>
+      <c r="A23" s="51"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="38"/>
+      <c r="U23" s="38"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="36"/>
+      <c r="Y23" s="36"/>
     </row>
     <row r="24" spans="1:25" s="10" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="S24" s="27" t="s">
+      <c r="S24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -1742,20 +1751,20 @@
     <mergeCell ref="X6:Y6"/>
     <mergeCell ref="A19:L23"/>
     <mergeCell ref="X7:Y13"/>
+    <mergeCell ref="S14:W14"/>
+    <mergeCell ref="A7:H13"/>
+    <mergeCell ref="A14:L14"/>
     <mergeCell ref="A2:Y2"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="J3:N3"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="S14:W14"/>
     <mergeCell ref="O3:Y3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="S4:T4"/>
-    <mergeCell ref="A7:H13"/>
-    <mergeCell ref="A14:L14"/>
     <mergeCell ref="S24:Y24"/>
     <mergeCell ref="I6:R6"/>
     <mergeCell ref="I7:R11"/>

</xml_diff>